<commit_message>
Database for 20180501 and later
</commit_message>
<xml_diff>
--- a/Issue summary -1.xlsx
+++ b/Issue summary -1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="82">
   <si>
     <t xml:space="preserve">Bugs</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t xml:space="preserve">Remove 'other' remove 'test control' default to select and enable free text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inconsistent with changes below.</t>
   </si>
   <si>
     <t xml:space="preserve">incorrect naming of data fields</t>
@@ -572,8 +575,8 @@
   </sheetPr>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -868,54 +871,59 @@
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="11" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="12" s="1" customFormat="true" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L11" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" s="1" customFormat="true" ht="65.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="10"/>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K12" s="1" t="s">
+      <c r="J12" s="9" t="s">
         <v>69</v>
       </c>
+      <c r="K12" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="L12" s="9"/>
     </row>
     <row r="13" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="L13" s="9"/>
     </row>
-    <row r="14" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="1" customFormat="true" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="10"/>
       <c r="H14" s="10"/>
-      <c r="I14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J14" s="1" t="s">
+      <c r="I14" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="J14" s="9" t="s">
         <v>75</v>
       </c>
+      <c r="K14" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L14" s="9"/>
     </row>
     <row r="15" s="1" customFormat="true" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="10"/>
@@ -924,22 +932,22 @@
         <v>7</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I16" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>